<commit_message>
Add link to translator
Add a link to an online document translator.
</commit_message>
<xml_diff>
--- a/2021-04-12to04-16 (A5) C53517 SoftMARS/01_BASEfiles/03_13v03_BASE_QuestionsAndModel.xlsx
+++ b/2021-04-12to04-16 (A5) C53517 SoftMARS/01_BASEfiles/03_13v03_BASE_QuestionsAndModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwjva\Documents\GitHub\CMMITools\2021-04-12to04-16 (A5) C53517 SoftMARS\01_BASEfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EF8E1F8-2E98-4EBE-8227-AFDC090AD30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B081C7-6850-41CA-9ADF-D58D736715C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D66F76D2-5ED4-4763-9F91-DFFB43C68A4F}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D66F76D2-5ED4-4763-9F91-DFFB43C68A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="41" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2075" uniqueCount="1038">
   <si>
     <t>CAR 3.2</t>
   </si>
@@ -3825,12 +3825,18 @@
   <si>
     <t>Small updates.</t>
   </si>
+  <si>
+    <t>https://www.onlinedoctranslator.com/en/translationform</t>
+  </si>
+  <si>
+    <t>Online document translator</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4018,6 +4024,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -4237,7 +4250,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4554,10 +4567,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4626,6 +4635,11 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -8437,86 +8451,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB5103A-01F5-47C8-86EE-0AFE1F3E6E49}">
   <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="118"/>
-    <col min="2" max="2" width="9.77734375" style="118" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.21875" style="118" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="118" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="118"/>
+    <col min="1" max="1" width="8.77734375" style="116"/>
+    <col min="2" max="2" width="9.77734375" style="116" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.21875" style="116" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="116" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="116"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="28.8">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="116" t="s">
         <v>1010</v>
       </c>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="116" t="s">
         <v>1011</v>
       </c>
-      <c r="C2" s="118" t="s">
+      <c r="C2" s="116" t="s">
         <v>1012</v>
       </c>
-      <c r="D2" s="118" t="s">
+      <c r="D2" s="116" t="s">
         <v>1013</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8">
-      <c r="A3" s="118">
+      <c r="A3" s="116">
         <v>8</v>
       </c>
-      <c r="B3" s="117">
+      <c r="B3" s="115">
         <v>44346</v>
       </c>
-      <c r="C3" s="118" t="s">
+      <c r="C3" s="116" t="s">
         <v>1009</v>
       </c>
-      <c r="D3" s="118" t="s">
+      <c r="D3" s="116" t="s">
         <v>1014</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="118">
+      <c r="A4" s="116">
         <v>10</v>
       </c>
-      <c r="B4" s="117">
+      <c r="B4" s="115">
         <v>44566</v>
       </c>
-      <c r="C4" s="118" t="s">
+      <c r="C4" s="116" t="s">
         <v>1029</v>
       </c>
-      <c r="D4" s="118" t="s">
+      <c r="D4" s="116" t="s">
         <v>1030</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="118">
+      <c r="A5" s="116">
         <v>12</v>
       </c>
-      <c r="B5" s="117">
+      <c r="B5" s="115">
         <v>44217</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="116" t="s">
         <v>1032</v>
       </c>
-      <c r="D5" s="118" t="s">
+      <c r="D5" s="116" t="s">
         <v>1031</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="118">
+      <c r="A6" s="116">
         <v>13</v>
       </c>
-      <c r="B6" s="117">
+      <c r="B6" s="115">
         <v>44667</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="116" t="s">
         <v>1035</v>
       </c>
-      <c r="D6" s="118" t="s">
+      <c r="D6" s="116" t="s">
         <v>1014</v>
       </c>
     </row>
@@ -17577,119 +17591,133 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7AA28D-0521-46F5-BE8B-9DA64F4C5175}">
-  <dimension ref="B2:C22"/>
+  <dimension ref="B2:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="16384" width="8.77734375" style="112"/>
+    <col min="1" max="16384" width="8.77734375" style="136"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="136" t="s">
         <v>981</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="C3" s="112" t="s">
+      <c r="C3" s="136" t="s">
         <v>982</v>
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="C4" s="112" t="s">
+      <c r="C4" s="136" t="s">
         <v>983</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="136" t="s">
         <v>1034</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="136" t="s">
         <v>984</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="136" t="s">
         <v>985</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="C8" s="112" t="s">
+      <c r="C8" s="136" t="s">
         <v>986</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="136" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="C10" s="112" t="s">
+      <c r="C10" s="136" t="s">
         <v>988</v>
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="136" t="s">
         <v>989</v>
       </c>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="112" t="s">
+      <c r="B13" s="136" t="s">
         <v>990</v>
       </c>
     </row>
     <row r="14" spans="2:3">
-      <c r="C14" s="112" t="s">
+      <c r="C14" s="136" t="s">
         <v>991</v>
       </c>
     </row>
     <row r="15" spans="2:3">
-      <c r="C15" s="113" t="s">
+      <c r="C15" s="137" t="s">
         <v>992</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="C16" s="113" t="s">
+      <c r="C16" s="137" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="112" t="s">
+    <row r="17" spans="2:3">
+      <c r="C17" s="136" t="s">
         <v>994</v>
       </c>
     </row>
-    <row r="18" spans="3:3">
-      <c r="C18" s="113" t="s">
+    <row r="18" spans="2:3">
+      <c r="C18" s="137" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="19" spans="3:3">
-      <c r="C19" s="113" t="s">
+    <row r="19" spans="2:3">
+      <c r="C19" s="137" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
-      <c r="C20" s="112" t="s">
+    <row r="20" spans="2:3">
+      <c r="C20" s="136" t="s">
         <v>997</v>
       </c>
     </row>
-    <row r="21" spans="3:3">
-      <c r="C21" s="112" t="s">
+    <row r="21" spans="2:3">
+      <c r="C21" s="136" t="s">
         <v>998</v>
       </c>
     </row>
-    <row r="22" spans="3:3">
-      <c r="C22" s="112" t="s">
+    <row r="22" spans="2:3">
+      <c r="C22" s="136" t="s">
         <v>999</v>
       </c>
     </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="136" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="C26" s="138" t="s">
+        <v>1036</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C26" r:id="rId1" xr:uid="{ED87D12A-1BF5-40C3-BC08-8F0F812EC584}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -27035,54 +27063,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:22" ht="93.6">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="125" t="s">
         <v>916</v>
       </c>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="125" t="s">
         <v>917</v>
       </c>
-      <c r="C2" s="125" t="s">
+      <c r="C2" s="123" t="s">
         <v>918</v>
       </c>
-      <c r="D2" s="125"/>
-      <c r="E2" s="126" t="s">
+      <c r="D2" s="123"/>
+      <c r="E2" s="124" t="s">
         <v>919</v>
       </c>
-      <c r="F2" s="126"/>
-      <c r="G2" s="125" t="s">
+      <c r="F2" s="124"/>
+      <c r="G2" s="123" t="s">
         <v>920</v>
       </c>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="126" t="s">
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="124" t="s">
         <v>921</v>
       </c>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="124"/>
       <c r="N2" s="61" t="s">
         <v>922</v>
       </c>
       <c r="O2" s="62" t="s">
         <v>923</v>
       </c>
-      <c r="P2" s="125" t="s">
+      <c r="P2" s="123" t="s">
         <v>924</v>
       </c>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
-      <c r="S2" s="126" t="s">
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="124" t="s">
         <v>925</v>
       </c>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
+      <c r="T2" s="124"/>
+      <c r="U2" s="124"/>
       <c r="V2" s="63" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.6">
-      <c r="A3" s="127"/>
-      <c r="B3" s="127"/>
+      <c r="A3" s="125"/>
+      <c r="B3" s="125"/>
       <c r="C3" s="65" t="s">
         <v>331</v>
       </c>
@@ -27145,7 +27173,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.6">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="122" t="s">
         <v>927</v>
       </c>
       <c r="B4" s="67" t="s">
@@ -27213,7 +27241,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.6">
-      <c r="A5" s="124"/>
+      <c r="A5" s="122"/>
       <c r="B5" s="66">
         <v>1.1000000000000001</v>
       </c>
@@ -27279,7 +27307,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.6">
-      <c r="A6" s="124"/>
+      <c r="A6" s="122"/>
       <c r="B6" s="66">
         <v>1.2</v>
       </c>
@@ -27319,7 +27347,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.6">
-      <c r="A7" s="124"/>
+      <c r="A7" s="122"/>
       <c r="B7" s="66">
         <v>1.3</v>
       </c>
@@ -27349,7 +27377,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.6">
-      <c r="A8" s="124"/>
+      <c r="A8" s="122"/>
       <c r="B8" s="66">
         <v>1.4</v>
       </c>
@@ -27377,7 +27405,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.6">
-      <c r="A9" s="124" t="s">
+      <c r="A9" s="122" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="67" t="s">
@@ -27443,7 +27471,7 @@
       <c r="V9" s="69"/>
     </row>
     <row r="10" spans="1:22" ht="15.6">
-      <c r="A10" s="124"/>
+      <c r="A10" s="122"/>
       <c r="B10" s="66">
         <v>2.1</v>
       </c>
@@ -27509,7 +27537,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.6">
-      <c r="A11" s="124"/>
+      <c r="A11" s="122"/>
       <c r="B11" s="66">
         <v>2.2000000000000002</v>
       </c>
@@ -27575,7 +27603,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.6">
-      <c r="A12" s="124"/>
+      <c r="A12" s="122"/>
       <c r="B12" s="66">
         <v>2.2999999999999998</v>
       </c>
@@ -27631,7 +27659,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.6">
-      <c r="A13" s="124"/>
+      <c r="A13" s="122"/>
       <c r="B13" s="66">
         <v>2.4</v>
       </c>
@@ -27679,7 +27707,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.6">
-      <c r="A14" s="124"/>
+      <c r="A14" s="122"/>
       <c r="B14" s="66">
         <v>2.5</v>
       </c>
@@ -27717,7 +27745,7 @@
       <c r="V14" s="69"/>
     </row>
     <row r="15" spans="1:22" ht="15.6">
-      <c r="A15" s="124"/>
+      <c r="A15" s="122"/>
       <c r="B15" s="66">
         <v>2.6</v>
       </c>
@@ -27753,7 +27781,7 @@
       <c r="V15" s="69"/>
     </row>
     <row r="16" spans="1:22" ht="15.6">
-      <c r="A16" s="124"/>
+      <c r="A16" s="122"/>
       <c r="B16" s="66">
         <v>2.7</v>
       </c>
@@ -27781,7 +27809,7 @@
       <c r="V16" s="69"/>
     </row>
     <row r="17" spans="1:22" ht="15.6">
-      <c r="A17" s="124"/>
+      <c r="A17" s="122"/>
       <c r="B17" s="66">
         <v>2.8</v>
       </c>
@@ -27809,7 +27837,7 @@
       <c r="V17" s="69"/>
     </row>
     <row r="18" spans="1:22" ht="15.6">
-      <c r="A18" s="124" t="s">
+      <c r="A18" s="122" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="67" t="s">
@@ -27873,7 +27901,7 @@
       <c r="V18" s="69"/>
     </row>
     <row r="19" spans="1:22" ht="15.6">
-      <c r="A19" s="124"/>
+      <c r="A19" s="122"/>
       <c r="B19" s="66">
         <v>3.1</v>
       </c>
@@ -27937,7 +27965,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.6">
-      <c r="A20" s="124"/>
+      <c r="A20" s="122"/>
       <c r="B20" s="66">
         <v>3.2</v>
       </c>
@@ -27995,7 +28023,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.6">
-      <c r="A21" s="124"/>
+      <c r="A21" s="122"/>
       <c r="B21" s="66">
         <v>3.3</v>
       </c>
@@ -28045,7 +28073,7 @@
       <c r="V21" s="69"/>
     </row>
     <row r="22" spans="1:22" ht="15.6">
-      <c r="A22" s="124"/>
+      <c r="A22" s="122"/>
       <c r="B22" s="66">
         <v>3.4</v>
       </c>
@@ -28091,7 +28119,7 @@
       <c r="V22" s="69"/>
     </row>
     <row r="23" spans="1:22" ht="15.6">
-      <c r="A23" s="124"/>
+      <c r="A23" s="122"/>
       <c r="B23" s="66">
         <v>3.5</v>
       </c>
@@ -28133,7 +28161,7 @@
       <c r="V23" s="69"/>
     </row>
     <row r="24" spans="1:22" ht="15.6">
-      <c r="A24" s="124"/>
+      <c r="A24" s="122"/>
       <c r="B24" s="66">
         <v>3.6</v>
       </c>
@@ -28171,7 +28199,7 @@
       <c r="V24" s="69"/>
     </row>
     <row r="25" spans="1:22" ht="15.6">
-      <c r="A25" s="124"/>
+      <c r="A25" s="122"/>
       <c r="B25" s="66">
         <v>3.7</v>
       </c>
@@ -28201,7 +28229,7 @@
       <c r="V25" s="69"/>
     </row>
     <row r="26" spans="1:22" ht="15.6">
-      <c r="A26" s="124" t="s">
+      <c r="A26" s="122" t="s">
         <v>931</v>
       </c>
       <c r="B26" s="67" t="s">
@@ -28239,7 +28267,7 @@
       <c r="V26" s="69"/>
     </row>
     <row r="27" spans="1:22" ht="15.6">
-      <c r="A27" s="124"/>
+      <c r="A27" s="122"/>
       <c r="B27" s="66">
         <v>4.0999999999999996</v>
       </c>
@@ -28277,7 +28305,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.6">
-      <c r="A28" s="124"/>
+      <c r="A28" s="122"/>
       <c r="B28" s="66">
         <v>4.2</v>
       </c>
@@ -28307,7 +28335,7 @@
       <c r="V28" s="69"/>
     </row>
     <row r="29" spans="1:22" ht="15.6">
-      <c r="A29" s="124"/>
+      <c r="A29" s="122"/>
       <c r="B29" s="66">
         <v>4.3</v>
       </c>
@@ -28335,7 +28363,7 @@
       <c r="V29" s="69"/>
     </row>
     <row r="30" spans="1:22" ht="15.6">
-      <c r="A30" s="124"/>
+      <c r="A30" s="122"/>
       <c r="B30" s="66">
         <v>4.4000000000000004</v>
       </c>
@@ -28363,7 +28391,7 @@
       <c r="V30" s="69"/>
     </row>
     <row r="31" spans="1:22" ht="15.6">
-      <c r="A31" s="124"/>
+      <c r="A31" s="122"/>
       <c r="B31" s="66">
         <v>4.5</v>
       </c>
@@ -28391,7 +28419,7 @@
       <c r="V31" s="69"/>
     </row>
     <row r="32" spans="1:22" ht="15.6">
-      <c r="A32" s="124" t="s">
+      <c r="A32" s="122" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="67" t="s">
@@ -28423,7 +28451,7 @@
       <c r="V32" s="69"/>
     </row>
     <row r="33" spans="1:22" ht="15.6">
-      <c r="A33" s="124"/>
+      <c r="A33" s="122"/>
       <c r="B33" s="66">
         <v>5.0999999999999996</v>
       </c>
@@ -28453,7 +28481,7 @@
       <c r="V33" s="69"/>
     </row>
     <row r="34" spans="1:22" ht="15.6">
-      <c r="A34" s="124"/>
+      <c r="A34" s="122"/>
       <c r="B34" s="66">
         <v>5.2</v>
       </c>
@@ -28481,7 +28509,7 @@
       <c r="V34" s="69"/>
     </row>
     <row r="35" spans="1:22" ht="15.6">
-      <c r="A35" s="124"/>
+      <c r="A35" s="122"/>
       <c r="B35" s="66">
         <v>5.3</v>
       </c>
@@ -28671,109 +28699,109 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="93.6">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="125" t="s">
         <v>916</v>
       </c>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="125" t="s">
         <v>917</v>
       </c>
-      <c r="C2" s="125" t="s">
+      <c r="C2" s="123" t="s">
         <v>918</v>
       </c>
-      <c r="D2" s="125"/>
-      <c r="E2" s="126" t="s">
+      <c r="D2" s="123"/>
+      <c r="E2" s="124" t="s">
         <v>919</v>
       </c>
-      <c r="F2" s="126"/>
-      <c r="G2" s="125" t="s">
+      <c r="F2" s="124"/>
+      <c r="G2" s="123" t="s">
         <v>920</v>
       </c>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="126" t="s">
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="124" t="s">
         <v>921</v>
       </c>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="124"/>
       <c r="N2" s="61" t="s">
         <v>922</v>
       </c>
       <c r="O2" s="62" t="s">
         <v>923</v>
       </c>
-      <c r="P2" s="125" t="s">
+      <c r="P2" s="123" t="s">
         <v>924</v>
       </c>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
-      <c r="S2" s="126" t="s">
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="124" t="s">
         <v>925</v>
       </c>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
+      <c r="T2" s="124"/>
+      <c r="U2" s="124"/>
       <c r="V2" s="63" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.6">
-      <c r="A3" s="127"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="119" t="s">
+      <c r="A3" s="125"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="117" t="s">
         <v>331</v>
       </c>
-      <c r="D3" s="119" t="s">
+      <c r="D3" s="117" t="s">
         <v>332</v>
       </c>
-      <c r="E3" s="120" t="s">
+      <c r="E3" s="118" t="s">
         <v>234</v>
       </c>
-      <c r="F3" s="120" t="s">
+      <c r="F3" s="118" t="s">
         <v>333</v>
       </c>
-      <c r="G3" s="119" t="s">
+      <c r="G3" s="117" t="s">
         <v>236</v>
       </c>
-      <c r="H3" s="119" t="s">
+      <c r="H3" s="117" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="119" t="s">
+      <c r="I3" s="117" t="s">
         <v>235</v>
       </c>
-      <c r="J3" s="119" t="s">
+      <c r="J3" s="117" t="s">
         <v>237</v>
       </c>
-      <c r="K3" s="120" t="s">
+      <c r="K3" s="118" t="s">
         <v>241</v>
       </c>
-      <c r="L3" s="120" t="s">
+      <c r="L3" s="118" t="s">
         <v>240</v>
       </c>
-      <c r="M3" s="120" t="s">
+      <c r="M3" s="118" t="s">
         <v>239</v>
       </c>
-      <c r="N3" s="119" t="s">
+      <c r="N3" s="117" t="s">
         <v>242</v>
       </c>
-      <c r="O3" s="120" t="s">
+      <c r="O3" s="118" t="s">
         <v>243</v>
       </c>
-      <c r="P3" s="119" t="s">
+      <c r="P3" s="117" t="s">
         <v>245</v>
       </c>
-      <c r="Q3" s="119" t="s">
+      <c r="Q3" s="117" t="s">
         <v>246</v>
       </c>
-      <c r="R3" s="119" t="s">
+      <c r="R3" s="117" t="s">
         <v>244</v>
       </c>
-      <c r="S3" s="120" t="s">
+      <c r="S3" s="118" t="s">
         <v>247</v>
       </c>
-      <c r="T3" s="120" t="s">
+      <c r="T3" s="118" t="s">
         <v>249</v>
       </c>
-      <c r="U3" s="120" t="s">
+      <c r="U3" s="118" t="s">
         <v>248</v>
       </c>
       <c r="V3" s="63" t="s">
@@ -28781,7 +28809,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.6">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="122" t="s">
         <v>927</v>
       </c>
       <c r="B4" s="67" t="s">
@@ -28849,8 +28877,8 @@
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.6">
-      <c r="A5" s="124"/>
-      <c r="B5" s="120">
+      <c r="A5" s="122"/>
+      <c r="B5" s="118">
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" s="70" t="s">
@@ -28915,8 +28943,8 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.6">
-      <c r="A6" s="124"/>
-      <c r="B6" s="120">
+      <c r="A6" s="122"/>
+      <c r="B6" s="118">
         <v>1.2</v>
       </c>
       <c r="C6" s="70"/>
@@ -28955,8 +28983,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.6">
-      <c r="A7" s="124"/>
-      <c r="B7" s="123">
+      <c r="A7" s="122"/>
+      <c r="B7" s="121">
         <v>1.3</v>
       </c>
       <c r="C7" s="70"/>
@@ -28985,8 +29013,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.6" hidden="1">
-      <c r="A8" s="124"/>
-      <c r="B8" s="120">
+      <c r="A8" s="122"/>
+      <c r="B8" s="118">
         <v>1.4</v>
       </c>
       <c r="C8" s="70"/>
@@ -29013,7 +29041,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.6">
-      <c r="A9" s="124" t="s">
+      <c r="A9" s="122" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="67" t="s">
@@ -29079,8 +29107,8 @@
       <c r="V9" s="69"/>
     </row>
     <row r="10" spans="1:22" ht="15.6">
-      <c r="A10" s="124"/>
-      <c r="B10" s="120">
+      <c r="A10" s="122"/>
+      <c r="B10" s="118">
         <v>2.1</v>
       </c>
       <c r="C10" s="70" t="s">
@@ -29145,8 +29173,8 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.6">
-      <c r="A11" s="124"/>
-      <c r="B11" s="120">
+      <c r="A11" s="122"/>
+      <c r="B11" s="118">
         <v>2.2000000000000002</v>
       </c>
       <c r="C11" s="70" t="s">
@@ -29211,8 +29239,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.6">
-      <c r="A12" s="124"/>
-      <c r="B12" s="120">
+      <c r="A12" s="122"/>
+      <c r="B12" s="118">
         <v>2.2999999999999998</v>
       </c>
       <c r="C12" s="70" t="s">
@@ -29267,8 +29295,8 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.6">
-      <c r="A13" s="124"/>
-      <c r="B13" s="120">
+      <c r="A13" s="122"/>
+      <c r="B13" s="118">
         <v>2.4</v>
       </c>
       <c r="C13" s="70" t="s">
@@ -29315,8 +29343,8 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.6">
-      <c r="A14" s="124"/>
-      <c r="B14" s="120">
+      <c r="A14" s="122"/>
+      <c r="B14" s="118">
         <v>2.5</v>
       </c>
       <c r="C14" s="70"/>
@@ -29353,8 +29381,8 @@
       <c r="V14" s="69"/>
     </row>
     <row r="15" spans="1:22" ht="15.6">
-      <c r="A15" s="124"/>
-      <c r="B15" s="120">
+      <c r="A15" s="122"/>
+      <c r="B15" s="118">
         <v>2.6</v>
       </c>
       <c r="C15" s="70"/>
@@ -29389,8 +29417,8 @@
       <c r="V15" s="69"/>
     </row>
     <row r="16" spans="1:22" ht="15.6">
-      <c r="A16" s="124"/>
-      <c r="B16" s="120">
+      <c r="A16" s="122"/>
+      <c r="B16" s="118">
         <v>2.7</v>
       </c>
       <c r="C16" s="70"/>
@@ -29417,8 +29445,8 @@
       <c r="V16" s="69"/>
     </row>
     <row r="17" spans="1:22" ht="15.6">
-      <c r="A17" s="124"/>
-      <c r="B17" s="120">
+      <c r="A17" s="122"/>
+      <c r="B17" s="118">
         <v>2.8</v>
       </c>
       <c r="C17" s="70"/>
@@ -29445,7 +29473,7 @@
       <c r="V17" s="69"/>
     </row>
     <row r="18" spans="1:22" ht="15.6">
-      <c r="A18" s="124" t="s">
+      <c r="A18" s="122" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="67" t="s">
@@ -29509,8 +29537,8 @@
       <c r="V18" s="69"/>
     </row>
     <row r="19" spans="1:22" ht="15.6">
-      <c r="A19" s="124"/>
-      <c r="B19" s="120">
+      <c r="A19" s="122"/>
+      <c r="B19" s="118">
         <v>3.1</v>
       </c>
       <c r="C19" s="70" t="s">
@@ -29573,8 +29601,8 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.6">
-      <c r="A20" s="124"/>
-      <c r="B20" s="120">
+      <c r="A20" s="122"/>
+      <c r="B20" s="118">
         <v>3.2</v>
       </c>
       <c r="C20" s="70" t="s">
@@ -29631,8 +29659,8 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.6">
-      <c r="A21" s="124"/>
-      <c r="B21" s="120">
+      <c r="A21" s="122"/>
+      <c r="B21" s="118">
         <v>3.3</v>
       </c>
       <c r="C21" s="70"/>
@@ -29681,8 +29709,8 @@
       <c r="V21" s="69"/>
     </row>
     <row r="22" spans="1:22" ht="15.6">
-      <c r="A22" s="124"/>
-      <c r="B22" s="120">
+      <c r="A22" s="122"/>
+      <c r="B22" s="118">
         <v>3.4</v>
       </c>
       <c r="C22" s="70"/>
@@ -29727,8 +29755,8 @@
       <c r="V22" s="69"/>
     </row>
     <row r="23" spans="1:22" ht="15.6">
-      <c r="A23" s="124"/>
-      <c r="B23" s="120">
+      <c r="A23" s="122"/>
+      <c r="B23" s="118">
         <v>3.5</v>
       </c>
       <c r="C23" s="70"/>
@@ -29769,8 +29797,8 @@
       <c r="V23" s="69"/>
     </row>
     <row r="24" spans="1:22" ht="15.6">
-      <c r="A24" s="124"/>
-      <c r="B24" s="120">
+      <c r="A24" s="122"/>
+      <c r="B24" s="118">
         <v>3.6</v>
       </c>
       <c r="C24" s="70"/>
@@ -29807,8 +29835,8 @@
       <c r="V24" s="69"/>
     </row>
     <row r="25" spans="1:22" ht="15.6">
-      <c r="A25" s="124"/>
-      <c r="B25" s="120">
+      <c r="A25" s="122"/>
+      <c r="B25" s="118">
         <v>3.7</v>
       </c>
       <c r="C25" s="70"/>
@@ -29837,7 +29865,7 @@
       <c r="V25" s="69"/>
     </row>
     <row r="26" spans="1:22" ht="15.6">
-      <c r="A26" s="124" t="s">
+      <c r="A26" s="122" t="s">
         <v>931</v>
       </c>
       <c r="B26" s="67" t="s">
@@ -29875,8 +29903,8 @@
       <c r="V26" s="69"/>
     </row>
     <row r="27" spans="1:22" ht="15.6">
-      <c r="A27" s="124"/>
-      <c r="B27" s="120">
+      <c r="A27" s="122"/>
+      <c r="B27" s="118">
         <v>4.0999999999999996</v>
       </c>
       <c r="C27" s="70" t="s">
@@ -29913,8 +29941,8 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.6">
-      <c r="A28" s="124"/>
-      <c r="B28" s="120">
+      <c r="A28" s="122"/>
+      <c r="B28" s="118">
         <v>4.2</v>
       </c>
       <c r="C28" s="70"/>
@@ -29943,8 +29971,8 @@
       <c r="V28" s="69"/>
     </row>
     <row r="29" spans="1:22" ht="15.6">
-      <c r="A29" s="124"/>
-      <c r="B29" s="120">
+      <c r="A29" s="122"/>
+      <c r="B29" s="118">
         <v>4.3</v>
       </c>
       <c r="C29" s="70"/>
@@ -29971,8 +29999,8 @@
       <c r="V29" s="69"/>
     </row>
     <row r="30" spans="1:22" ht="15.6">
-      <c r="A30" s="124"/>
-      <c r="B30" s="120">
+      <c r="A30" s="122"/>
+      <c r="B30" s="118">
         <v>4.4000000000000004</v>
       </c>
       <c r="C30" s="70"/>
@@ -29999,8 +30027,8 @@
       <c r="V30" s="69"/>
     </row>
     <row r="31" spans="1:22" ht="15.6">
-      <c r="A31" s="124"/>
-      <c r="B31" s="120">
+      <c r="A31" s="122"/>
+      <c r="B31" s="118">
         <v>4.5</v>
       </c>
       <c r="C31" s="70"/>
@@ -30027,7 +30055,7 @@
       <c r="V31" s="69"/>
     </row>
     <row r="32" spans="1:22" ht="15.6">
-      <c r="A32" s="124" t="s">
+      <c r="A32" s="122" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="67" t="s">
@@ -30059,8 +30087,8 @@
       <c r="V32" s="69"/>
     </row>
     <row r="33" spans="1:22" ht="15.6">
-      <c r="A33" s="124"/>
-      <c r="B33" s="120">
+      <c r="A33" s="122"/>
+      <c r="B33" s="118">
         <v>5.0999999999999996</v>
       </c>
       <c r="C33" s="70"/>
@@ -30089,8 +30117,8 @@
       <c r="V33" s="69"/>
     </row>
     <row r="34" spans="1:22" ht="15.6">
-      <c r="A34" s="124"/>
-      <c r="B34" s="120">
+      <c r="A34" s="122"/>
+      <c r="B34" s="118">
         <v>5.2</v>
       </c>
       <c r="C34" s="70"/>
@@ -30117,8 +30145,8 @@
       <c r="V34" s="69"/>
     </row>
     <row r="35" spans="1:22" ht="15.6">
-      <c r="A35" s="124"/>
-      <c r="B35" s="120">
+      <c r="A35" s="122"/>
+      <c r="B35" s="118">
         <v>5.3</v>
       </c>
       <c r="C35" s="70"/>
@@ -30272,7 +30300,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="18">
-      <c r="A43" s="116" t="s">
+      <c r="A43" s="114" t="s">
         <v>1007</v>
       </c>
       <c r="C43" s="82"/>
@@ -30292,61 +30320,61 @@
       <c r="R43" s="82"/>
     </row>
     <row r="45" spans="1:22" ht="15.6">
-      <c r="C45" s="121" t="s">
+      <c r="C45" s="119" t="s">
         <v>247</v>
       </c>
-      <c r="D45" s="121" t="s">
+      <c r="D45" s="119" t="s">
         <v>248</v>
       </c>
-      <c r="E45" s="122" t="s">
+      <c r="E45" s="120" t="s">
         <v>249</v>
       </c>
-      <c r="F45" s="122" t="s">
+      <c r="F45" s="120" t="s">
         <v>244</v>
       </c>
-      <c r="G45" s="121" t="s">
+      <c r="G45" s="119" t="s">
         <v>331</v>
       </c>
-      <c r="H45" s="121" t="s">
+      <c r="H45" s="119" t="s">
         <v>332</v>
       </c>
-      <c r="I45" s="121" t="s">
+      <c r="I45" s="119" t="s">
         <v>245</v>
       </c>
-      <c r="J45" s="121" t="s">
+      <c r="J45" s="119" t="s">
         <v>239</v>
       </c>
-      <c r="K45" s="122" t="s">
+      <c r="K45" s="120" t="s">
         <v>243</v>
       </c>
-      <c r="L45" s="122" t="s">
+      <c r="L45" s="120" t="s">
         <v>240</v>
       </c>
-      <c r="M45" s="122" t="s">
+      <c r="M45" s="120" t="s">
         <v>241</v>
       </c>
-      <c r="N45" s="121" t="s">
+      <c r="N45" s="119" t="s">
         <v>333</v>
       </c>
-      <c r="O45" s="122" t="s">
+      <c r="O45" s="120" t="s">
         <v>246</v>
       </c>
-      <c r="P45" s="121" t="s">
+      <c r="P45" s="119" t="s">
         <v>235</v>
       </c>
-      <c r="Q45" s="121" t="s">
+      <c r="Q45" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="R45" s="121" t="s">
+      <c r="R45" s="119" t="s">
         <v>237</v>
       </c>
-      <c r="S45" s="122" t="s">
+      <c r="S45" s="120" t="s">
         <v>242</v>
       </c>
-      <c r="T45" s="122" t="s">
+      <c r="T45" s="120" t="s">
         <v>234</v>
       </c>
-      <c r="U45" s="122" t="s">
+      <c r="U45" s="120" t="s">
         <v>238</v>
       </c>
       <c r="V45" s="63" t="s">
@@ -30354,7 +30382,7 @@
       </c>
     </row>
     <row r="46" spans="1:22">
-      <c r="A46" s="124" t="s">
+      <c r="A46" s="122" t="s">
         <v>927</v>
       </c>
       <c r="B46" s="67" t="s">
@@ -30442,8 +30470,8 @@
       </c>
     </row>
     <row r="47" spans="1:22">
-      <c r="A47" s="124"/>
-      <c r="B47" s="120">
+      <c r="A47" s="122"/>
+      <c r="B47" s="118">
         <v>1.1000000000000001</v>
       </c>
       <c r="C47" s="68" t="str">
@@ -30528,8 +30556,8 @@
       </c>
     </row>
     <row r="48" spans="1:22">
-      <c r="A48" s="124"/>
-      <c r="B48" s="120">
+      <c r="A48" s="122"/>
+      <c r="B48" s="118">
         <v>1.2</v>
       </c>
       <c r="C48" s="68"/>
@@ -30575,8 +30603,8 @@
       </c>
     </row>
     <row r="49" spans="1:22">
-      <c r="A49" s="124"/>
-      <c r="B49" s="120">
+      <c r="A49" s="122"/>
+      <c r="B49" s="118">
         <v>1.3</v>
       </c>
       <c r="C49" s="68"/>
@@ -30607,7 +30635,7 @@
       </c>
     </row>
     <row r="50" spans="1:22">
-      <c r="A50" s="124" t="s">
+      <c r="A50" s="122" t="s">
         <v>5</v>
       </c>
       <c r="B50" s="67" t="s">
@@ -30692,8 +30720,8 @@
       <c r="V50" s="68"/>
     </row>
     <row r="51" spans="1:22">
-      <c r="A51" s="124"/>
-      <c r="B51" s="120">
+      <c r="A51" s="122"/>
+      <c r="B51" s="118">
         <v>2.1</v>
       </c>
       <c r="C51" s="68" t="str">
@@ -30778,8 +30806,8 @@
       </c>
     </row>
     <row r="52" spans="1:22">
-      <c r="A52" s="124"/>
-      <c r="B52" s="120">
+      <c r="A52" s="122"/>
+      <c r="B52" s="118">
         <v>2.2000000000000002</v>
       </c>
       <c r="C52" s="68" t="str">
@@ -30864,8 +30892,8 @@
       </c>
     </row>
     <row r="53" spans="1:22">
-      <c r="A53" s="124"/>
-      <c r="B53" s="120">
+      <c r="A53" s="122"/>
+      <c r="B53" s="118">
         <v>2.2999999999999998</v>
       </c>
       <c r="C53" s="68"/>
@@ -30935,8 +30963,8 @@
       </c>
     </row>
     <row r="54" spans="1:22">
-      <c r="A54" s="124"/>
-      <c r="B54" s="120">
+      <c r="A54" s="122"/>
+      <c r="B54" s="118">
         <v>2.4</v>
       </c>
       <c r="C54" s="68"/>
@@ -30994,8 +31022,8 @@
       </c>
     </row>
     <row r="55" spans="1:22">
-      <c r="A55" s="124"/>
-      <c r="B55" s="120">
+      <c r="A55" s="122"/>
+      <c r="B55" s="118">
         <v>2.5</v>
       </c>
       <c r="C55" s="68"/>
@@ -31038,8 +31066,8 @@
       <c r="V55" s="68"/>
     </row>
     <row r="56" spans="1:22">
-      <c r="A56" s="124"/>
-      <c r="B56" s="120">
+      <c r="A56" s="122"/>
+      <c r="B56" s="118">
         <v>2.6</v>
       </c>
       <c r="C56" s="68"/>
@@ -31079,8 +31107,8 @@
       <c r="V56" s="68"/>
     </row>
     <row r="57" spans="1:22">
-      <c r="A57" s="124"/>
-      <c r="B57" s="120">
+      <c r="A57" s="122"/>
+      <c r="B57" s="118">
         <v>2.7</v>
       </c>
       <c r="C57" s="68"/>
@@ -31108,8 +31136,8 @@
       <c r="V57" s="68"/>
     </row>
     <row r="58" spans="1:22">
-      <c r="A58" s="124"/>
-      <c r="B58" s="120">
+      <c r="A58" s="122"/>
+      <c r="B58" s="118">
         <v>2.8</v>
       </c>
       <c r="C58" s="68"/>
@@ -31137,7 +31165,7 @@
       <c r="V58" s="68"/>
     </row>
     <row r="59" spans="1:22">
-      <c r="A59" s="124" t="s">
+      <c r="A59" s="122" t="s">
         <v>2</v>
       </c>
       <c r="B59" s="67" t="s">
@@ -31222,8 +31250,8 @@
       </c>
     </row>
     <row r="60" spans="1:22">
-      <c r="A60" s="124"/>
-      <c r="B60" s="120">
+      <c r="A60" s="122"/>
+      <c r="B60" s="118">
         <v>3.1</v>
       </c>
       <c r="C60" s="68" t="str">
@@ -31305,8 +31333,8 @@
       </c>
     </row>
     <row r="61" spans="1:22">
-      <c r="A61" s="124"/>
-      <c r="B61" s="120">
+      <c r="A61" s="122"/>
+      <c r="B61" s="118">
         <v>3.2</v>
       </c>
       <c r="C61" s="68" t="str">
@@ -31379,8 +31407,8 @@
       </c>
     </row>
     <row r="62" spans="1:22">
-      <c r="A62" s="124"/>
-      <c r="B62" s="120">
+      <c r="A62" s="122"/>
+      <c r="B62" s="118">
         <v>3.3</v>
       </c>
       <c r="C62" s="68" t="str">
@@ -31441,8 +31469,8 @@
       <c r="V62" s="68"/>
     </row>
     <row r="63" spans="1:22">
-      <c r="A63" s="124"/>
-      <c r="B63" s="120">
+      <c r="A63" s="122"/>
+      <c r="B63" s="118">
         <v>3.4</v>
       </c>
       <c r="C63" s="68" t="str">
@@ -31497,8 +31525,8 @@
       <c r="V63" s="68"/>
     </row>
     <row r="64" spans="1:22">
-      <c r="A64" s="124"/>
-      <c r="B64" s="120">
+      <c r="A64" s="122"/>
+      <c r="B64" s="118">
         <v>3.5</v>
       </c>
       <c r="C64" s="68" t="str">
@@ -31547,8 +31575,8 @@
       <c r="V64" s="68"/>
     </row>
     <row r="65" spans="1:22">
-      <c r="A65" s="124"/>
-      <c r="B65" s="120">
+      <c r="A65" s="122"/>
+      <c r="B65" s="118">
         <v>3.6</v>
       </c>
       <c r="C65" s="68"/>
@@ -31591,8 +31619,8 @@
       <c r="V65" s="68"/>
     </row>
     <row r="66" spans="1:22">
-      <c r="A66" s="124"/>
-      <c r="B66" s="120">
+      <c r="A66" s="122"/>
+      <c r="B66" s="118">
         <v>3.7</v>
       </c>
       <c r="C66" s="68"/>
@@ -31623,7 +31651,7 @@
       <c r="V66" s="68"/>
     </row>
     <row r="67" spans="1:22">
-      <c r="A67" s="124" t="s">
+      <c r="A67" s="122" t="s">
         <v>931</v>
       </c>
       <c r="B67" s="67" t="s">
@@ -31666,8 +31694,8 @@
       <c r="V67" s="68"/>
     </row>
     <row r="68" spans="1:22">
-      <c r="A68" s="124"/>
-      <c r="B68" s="120">
+      <c r="A68" s="122"/>
+      <c r="B68" s="118">
         <v>4.0999999999999996</v>
       </c>
       <c r="C68" s="68" t="str">
@@ -31710,8 +31738,8 @@
       </c>
     </row>
     <row r="69" spans="1:22">
-      <c r="A69" s="124"/>
-      <c r="B69" s="120">
+      <c r="A69" s="122"/>
+      <c r="B69" s="118">
         <v>4.2</v>
       </c>
       <c r="C69" s="68" t="str">
@@ -31742,8 +31770,8 @@
       <c r="V69" s="68"/>
     </row>
     <row r="70" spans="1:22">
-      <c r="A70" s="124"/>
-      <c r="B70" s="120">
+      <c r="A70" s="122"/>
+      <c r="B70" s="118">
         <v>4.3</v>
       </c>
       <c r="C70" s="68"/>
@@ -31771,8 +31799,8 @@
       <c r="V70" s="68"/>
     </row>
     <row r="71" spans="1:22">
-      <c r="A71" s="124"/>
-      <c r="B71" s="120">
+      <c r="A71" s="122"/>
+      <c r="B71" s="118">
         <v>4.4000000000000004</v>
       </c>
       <c r="C71" s="68"/>
@@ -31800,8 +31828,8 @@
       <c r="V71" s="68"/>
     </row>
     <row r="72" spans="1:22">
-      <c r="A72" s="124"/>
-      <c r="B72" s="120">
+      <c r="A72" s="122"/>
+      <c r="B72" s="118">
         <v>4.5</v>
       </c>
       <c r="C72" s="68"/>
@@ -31829,7 +31857,7 @@
       <c r="V72" s="68"/>
     </row>
     <row r="73" spans="1:22">
-      <c r="A73" s="124" t="s">
+      <c r="A73" s="122" t="s">
         <v>17</v>
       </c>
       <c r="B73" s="67" t="s">
@@ -31863,8 +31891,8 @@
       <c r="V73" s="68"/>
     </row>
     <row r="74" spans="1:22">
-      <c r="A74" s="124"/>
-      <c r="B74" s="120">
+      <c r="A74" s="122"/>
+      <c r="B74" s="118">
         <v>5.0999999999999996</v>
       </c>
       <c r="C74" s="68" t="str">
@@ -31895,8 +31923,8 @@
       <c r="V74" s="68"/>
     </row>
     <row r="75" spans="1:22">
-      <c r="A75" s="124"/>
-      <c r="B75" s="120">
+      <c r="A75" s="122"/>
+      <c r="B75" s="118">
         <v>5.2</v>
       </c>
       <c r="C75" s="68"/>
@@ -31924,8 +31952,8 @@
       <c r="V75" s="68"/>
     </row>
     <row r="76" spans="1:22">
-      <c r="A76" s="124"/>
-      <c r="B76" s="120">
+      <c r="A76" s="122"/>
+      <c r="B76" s="118">
         <v>5.3</v>
       </c>
       <c r="C76" s="68"/>
@@ -31954,24 +31982,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:M2"/>
     <mergeCell ref="A46:A49"/>
     <mergeCell ref="A50:A58"/>
     <mergeCell ref="A59:A66"/>
     <mergeCell ref="A67:A72"/>
     <mergeCell ref="A73:A76"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A9:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="A32:A35"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:V35">
     <cfRule type="cellIs" dxfId="259" priority="151" operator="equal">
@@ -32546,10 +32574,10 @@
       <c r="R1" s="79"/>
     </row>
     <row r="2" spans="1:18" ht="68.099999999999994" customHeight="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="125" t="s">
         <v>916</v>
       </c>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="125" t="s">
         <v>917</v>
       </c>
       <c r="C2" s="65" t="s">
@@ -32600,8 +32628,8 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="127"/>
-      <c r="B3" s="127"/>
+      <c r="A3" s="125"/>
+      <c r="B3" s="125"/>
       <c r="C3" s="65" t="s">
         <v>331</v>
       </c>
@@ -32639,7 +32667,7 @@
       <c r="O3" s="65" t="s">
         <v>332</v>
       </c>
-      <c r="P3" s="114" t="s">
+      <c r="P3" s="112" t="s">
         <v>332</v>
       </c>
       <c r="Q3" s="65" t="s">
@@ -32650,7 +32678,7 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="122" t="s">
         <v>927</v>
       </c>
       <c r="B4" s="67" t="s">
@@ -32674,7 +32702,7 @@
       <c r="R4" s="81"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="124"/>
+      <c r="A5" s="122"/>
       <c r="B5" s="66">
         <v>1.1000000000000001</v>
       </c>
@@ -32726,7 +32754,7 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="124"/>
+      <c r="A6" s="122"/>
       <c r="B6" s="66">
         <v>1.2</v>
       </c>
@@ -32748,7 +32776,7 @@
       <c r="R6" s="67"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="124"/>
+      <c r="A7" s="122"/>
       <c r="B7" s="66">
         <v>1.3</v>
       </c>
@@ -32770,7 +32798,7 @@
       <c r="R7" s="67"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="124" t="s">
+      <c r="A8" s="122" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="67" t="s">
@@ -32794,7 +32822,7 @@
       <c r="R8" s="81"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="124"/>
+      <c r="A9" s="122"/>
       <c r="B9" s="66">
         <v>2.1</v>
       </c>
@@ -32846,7 +32874,7 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="124"/>
+      <c r="A10" s="122"/>
       <c r="B10" s="66">
         <v>2.2000000000000002</v>
       </c>
@@ -32898,7 +32926,7 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="124"/>
+      <c r="A11" s="122"/>
       <c r="B11" s="66">
         <v>2.2999999999999998</v>
       </c>
@@ -32934,7 +32962,7 @@
       <c r="R11" s="67"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="124"/>
+      <c r="A12" s="122"/>
       <c r="B12" s="66">
         <v>2.4</v>
       </c>
@@ -32970,7 +32998,7 @@
       <c r="R12" s="67"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="124"/>
+      <c r="A13" s="122"/>
       <c r="B13" s="66">
         <v>2.5</v>
       </c>
@@ -32992,7 +33020,7 @@
       <c r="R13" s="67"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="124"/>
+      <c r="A14" s="122"/>
       <c r="B14" s="66">
         <v>2.6</v>
       </c>
@@ -33014,7 +33042,7 @@
       <c r="R14" s="67"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="124"/>
+      <c r="A15" s="122"/>
       <c r="B15" s="66">
         <v>2.7</v>
       </c>
@@ -33036,7 +33064,7 @@
       <c r="R15" s="67"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="124"/>
+      <c r="A16" s="122"/>
       <c r="B16" s="66">
         <v>2.8</v>
       </c>
@@ -33058,7 +33086,7 @@
       <c r="R16" s="67"/>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="124" t="s">
+      <c r="A17" s="122" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="67" t="s">
@@ -33082,7 +33110,7 @@
       <c r="R17" s="81"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="124"/>
+      <c r="A18" s="122"/>
       <c r="B18" s="66">
         <v>3.1</v>
       </c>
@@ -33134,7 +33162,7 @@
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="124"/>
+      <c r="A19" s="122"/>
       <c r="B19" s="66">
         <v>3.2</v>
       </c>
@@ -33186,7 +33214,7 @@
       </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="124"/>
+      <c r="A20" s="122"/>
       <c r="B20" s="66">
         <v>3.3</v>
       </c>
@@ -33224,7 +33252,7 @@
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="124"/>
+      <c r="A21" s="122"/>
       <c r="B21" s="66">
         <v>3.4</v>
       </c>
@@ -33246,7 +33274,7 @@
       <c r="R21" s="67"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="124"/>
+      <c r="A22" s="122"/>
       <c r="B22" s="66">
         <v>3.5</v>
       </c>
@@ -33268,7 +33296,7 @@
       <c r="R22" s="67"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="124"/>
+      <c r="A23" s="122"/>
       <c r="B23" s="66">
         <v>3.6</v>
       </c>
@@ -33290,7 +33318,7 @@
       <c r="R23" s="67"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="124"/>
+      <c r="A24" s="122"/>
       <c r="B24" s="66">
         <v>3.7</v>
       </c>
@@ -33312,7 +33340,7 @@
       <c r="R24" s="67"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="124" t="s">
+      <c r="A25" s="122" t="s">
         <v>931</v>
       </c>
       <c r="B25" s="67" t="s">
@@ -33336,7 +33364,7 @@
       <c r="R25" s="81"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="124"/>
+      <c r="A26" s="122"/>
       <c r="B26" s="66">
         <v>4.0999999999999996</v>
       </c>
@@ -33372,7 +33400,7 @@
       <c r="R26" s="67"/>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="124"/>
+      <c r="A27" s="122"/>
       <c r="B27" s="66">
         <v>4.2</v>
       </c>
@@ -33394,7 +33422,7 @@
       <c r="R27" s="67"/>
     </row>
     <row r="28" spans="1:18">
-      <c r="A28" s="124"/>
+      <c r="A28" s="122"/>
       <c r="B28" s="66">
         <v>4.3</v>
       </c>
@@ -33416,7 +33444,7 @@
       <c r="R28" s="67"/>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="124"/>
+      <c r="A29" s="122"/>
       <c r="B29" s="66">
         <v>4.4000000000000004</v>
       </c>
@@ -33438,7 +33466,7 @@
       <c r="R29" s="67"/>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="124"/>
+      <c r="A30" s="122"/>
       <c r="B30" s="66">
         <v>4.5</v>
       </c>
@@ -33460,7 +33488,7 @@
       <c r="R30" s="67"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="124" t="s">
+      <c r="A31" s="122" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="67" t="s">
@@ -33484,7 +33512,7 @@
       <c r="R31" s="67"/>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="124"/>
+      <c r="A32" s="122"/>
       <c r="B32" s="66">
         <v>5.0999999999999996</v>
       </c>
@@ -33506,7 +33534,7 @@
       <c r="R32" s="67"/>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="124"/>
+      <c r="A33" s="122"/>
       <c r="B33" s="66">
         <v>5.2</v>
       </c>
@@ -33528,7 +33556,7 @@
       <c r="R33" s="67"/>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="124"/>
+      <c r="A34" s="122"/>
       <c r="B34" s="66">
         <v>5.3</v>
       </c>
@@ -33550,12 +33578,12 @@
       <c r="R34" s="67"/>
     </row>
     <row r="38" spans="1:18" ht="15.6">
-      <c r="A38" s="115" t="s">
+      <c r="A38" s="113" t="s">
         <v>1006</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.6">
-      <c r="A39" s="115" t="s">
+      <c r="A39" s="113" t="s">
         <v>1008</v>
       </c>
     </row>
@@ -34018,14 +34046,14 @@
       <c r="B4" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="128" t="s">
+      <c r="C4" s="126" t="s">
         <v>962</v>
       </c>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
       <c r="I4" s="4" t="s">
         <v>963</v>
       </c>
@@ -34049,17 +34077,17 @@
       <c r="B5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="129" t="s">
+      <c r="C5" s="127" t="s">
         <v>965</v>
       </c>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="130"/>
-      <c r="K5" s="131"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="129"/>
       <c r="L5" s="94"/>
       <c r="M5" s="94"/>
       <c r="N5" s="94"/>
@@ -34074,13 +34102,13 @@
       <c r="B6" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="132" t="s">
+      <c r="C6" s="130" t="s">
         <v>967</v>
       </c>
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="G6" s="134"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="132"/>
       <c r="H6" s="102" t="s">
         <v>968</v>
       </c>
@@ -34140,14 +34168,14 @@
       <c r="B19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="128" t="s">
+      <c r="C19" s="126" t="s">
         <v>962</v>
       </c>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="128"/>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
+      <c r="H19" s="126"/>
       <c r="I19" s="4" t="s">
         <v>963</v>
       </c>
@@ -34160,9 +34188,9 @@
       <c r="L19" s="98"/>
       <c r="M19" s="98"/>
       <c r="N19" s="98"/>
-      <c r="O19" s="135"/>
-      <c r="P19" s="136"/>
-      <c r="Q19" s="137"/>
+      <c r="O19" s="133"/>
+      <c r="P19" s="134"/>
+      <c r="Q19" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -35413,6 +35441,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F513751AC33344AB32CFD2920EFE649" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f6feadb6ddc3dd981964989ee73899f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="72e3a154-4955-46c3-9573-e9dec3e1f195" xmlns:ns3="ec500478-62e0-46fc-87f1-cfa988e486b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b71de754eeec595e1494c9b2c7a90b" ns2:_="" ns3:_="">
     <xsd:import namespace="72e3a154-4955-46c3-9573-e9dec3e1f195"/>
@@ -35629,36 +35672,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A66621A-BA41-4919-8299-0C0501A99E42}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50C3019A-A66F-442E-9D7D-BA1B50D45000}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="72e3a154-4955-46c3-9573-e9dec3e1f195"/>
-    <ds:schemaRef ds:uri="ec500478-62e0-46fc-87f1-cfa988e486b4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -35681,9 +35698,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50C3019A-A66F-442E-9D7D-BA1B50D45000}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A66621A-BA41-4919-8299-0C0501A99E42}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="72e3a154-4955-46c3-9573-e9dec3e1f195"/>
+    <ds:schemaRef ds:uri="ec500478-62e0-46fc-87f1-cfa988e486b4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>